<commit_message>
commit new changes in verifyDeleteSearch
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omar\Glance Project Docs\GlanceAutomation\GlanceAutomationTests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15015" windowHeight="5985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ChartData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:O17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -425,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="A1:K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
commit test cases _ Sachini
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,15 +3,26 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sachini\Glance\Glance Automation\GlanceAutomationTests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15015" windowHeight="5985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15015" windowHeight="5985" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ChartData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="EntityData" sheetId="3" r:id="rId3"/>
+    <sheet name="DateRange" sheetId="4" r:id="rId4"/>
+    <sheet name="EngagementData" sheetId="5" r:id="rId5"/>
+    <sheet name="SearchData" sheetId="6" r:id="rId6"/>
+    <sheet name="SQLData" sheetId="7" r:id="rId7"/>
+    <sheet name="DeleteSearchData" sheetId="8" r:id="rId8"/>
+    <sheet name="ShowEntryData" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>Metric</t>
   </si>
@@ -102,6 +113,111 @@
   </si>
   <si>
     <t>Affinion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entity </t>
+  </si>
+  <si>
+    <t>Engagement</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>Yesterday</t>
+  </si>
+  <si>
+    <t>Last 7 days</t>
+  </si>
+  <si>
+    <t>Last 30 days</t>
+  </si>
+  <si>
+    <t>This Month</t>
+  </si>
+  <si>
+    <t>Last Month</t>
+  </si>
+  <si>
+    <t>Custom</t>
+  </si>
+  <si>
+    <t>EngagementName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years </t>
+  </si>
+  <si>
+    <t>DeliveryMethod</t>
+  </si>
+  <si>
+    <t>ContractType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account </t>
+  </si>
+  <si>
+    <t>AVA</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>SQL search</t>
+  </si>
+  <si>
+    <t>SELECT * FROM accounts;</t>
+  </si>
+  <si>
+    <t>SELECT * FROM account</t>
+  </si>
+  <si>
+    <t>EntityID</t>
+  </si>
+  <si>
+    <t>EntityName</t>
+  </si>
+  <si>
+    <t>Home TV</t>
+  </si>
+  <si>
+    <t>ShowEntry</t>
+  </si>
+  <si>
+    <t>DateRange</t>
+  </si>
+  <si>
+    <t>Utility</t>
+  </si>
+  <si>
+    <t>Capacity Based</t>
+  </si>
+  <si>
+    <t>Engagement1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -137,8 +253,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,4 +784,309 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>